<commit_message>
some changes related to Driver Master upload
</commit_message>
<xml_diff>
--- a/src/assets/Download/DriverMasterTemplate.xlsx
+++ b/src/assets/Download/DriverMasterTemplate.xlsx
@@ -4,28 +4,35 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7650"/>
+    <workbookView windowWidth="19635" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
-  <si>
-    <t>ManualDriverCode</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>DriverName</t>
   </si>
   <si>
     <t>LicenseNo</t>
-  </si>
-  <si>
-    <t>LicenseValidityDate</t>
   </si>
   <si>
     <t>CountryCode</t>
@@ -46,25 +53,13 @@
     <t>AssignedVehicleNo</t>
   </si>
   <si>
-    <t>DateofBirth</t>
-  </si>
-  <si>
-    <t>Active</t>
-  </si>
-  <si>
-    <t>DR0001</t>
-  </si>
-  <si>
     <t>Sohan Sharma</t>
   </si>
   <si>
     <t>MH0523565478978</t>
   </si>
   <si>
-    <t>31-03-2024</t>
-  </si>
-  <si>
-    <t>91 : India</t>
+    <t>India</t>
   </si>
   <si>
     <t>Near Andheri Metro Station, Mumbai</t>
@@ -75,24 +70,18 @@
   <si>
     <t>MH05AA4444</t>
   </si>
-  <si>
-    <t>21-01-1990</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -108,9 +97,15 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri Light"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri Light"/>
       <charset val="134"/>
     </font>
     <font>
@@ -267,8 +262,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.149998474074526"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
     <fill>
@@ -584,133 +579,133 @@
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -720,7 +715,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1254,13 +1249,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="7"/>
   <cols>
     <col min="1" max="1" width="22.7142857142857" customWidth="1"/>
     <col min="2" max="2" width="16.2857142857143" customWidth="1"/>
@@ -1269,14 +1264,10 @@
     <col min="5" max="5" width="16.2857142857143" customWidth="1"/>
     <col min="6" max="6" width="13.2857142857143" customWidth="1"/>
     <col min="7" max="7" width="37.8571428571429" customWidth="1"/>
-    <col min="8" max="8" width="11" customWidth="1"/>
-    <col min="9" max="9" width="8.85714285714286" customWidth="1"/>
-    <col min="10" max="10" width="22.5714285714286" customWidth="1"/>
-    <col min="11" max="11" width="13.7142857142857" customWidth="1"/>
-    <col min="12" max="12" width="8.42857142857143" customWidth="1"/>
+    <col min="8" max="8" width="19.1428571428571" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:12">
+    <row r="1" s="1" customFormat="1" spans="1:8">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1301,55 +1292,31 @@
       <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+    </row>
+    <row r="2" s="1" customFormat="1" spans="1:8">
+      <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="D2" s="3">
+        <v>9311555369</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" s="1" customFormat="1" ht="14.25" spans="1:12">
-      <c r="A2" s="1" t="s">
+      <c r="F2" s="3">
+        <v>400016</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="H2" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" s="1">
-        <v>9311555369</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" s="1">
-        <v>400016</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
some changes regarding to WT-548
</commit_message>
<xml_diff>
--- a/src/assets/Download/DriverMasterTemplate.xlsx
+++ b/src/assets/Download/DriverMasterTemplate.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>DriverName</t>
   </si>
@@ -35,6 +35,9 @@
     <t>LicenseNo</t>
   </si>
   <si>
+    <t>LicenseValidityDate</t>
+  </si>
+  <si>
     <t>CountryCode</t>
   </si>
   <si>
@@ -50,6 +53,9 @@
     <t>City</t>
   </si>
   <si>
+    <t>DateofBirth</t>
+  </si>
+  <si>
     <t>AssignedVehicleNo</t>
   </si>
   <si>
@@ -59,10 +65,19 @@
     <t>MH0523565478978</t>
   </si>
   <si>
+    <t>1/3/2024</t>
+  </si>
+  <si>
     <t>India</t>
   </si>
   <si>
+    <t>9311555369</t>
+  </si>
+  <si>
     <t>Near Andheri Metro Station, Mumbai</t>
+  </si>
+  <si>
+    <t>400016</t>
   </si>
   <si>
     <t>Mumbai</t>
@@ -81,19 +96,13 @@
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="134"/>
     </font>
     <font>
       <b/>
@@ -579,133 +588,133 @@
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -713,9 +722,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1249,13 +1258,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1"/>
   <cols>
     <col min="1" max="1" width="22.7142857142857" customWidth="1"/>
     <col min="2" max="2" width="16.2857142857143" customWidth="1"/>
@@ -1267,56 +1276,68 @@
     <col min="8" max="8" width="19.1428571428571" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:8">
-      <c r="A1" s="2" t="s">
+    <row r="1" customFormat="1" spans="1:10">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" s="1" customFormat="1" spans="1:8">
-      <c r="A2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>9</v>
+    <row r="2" customFormat="1" spans="1:10">
+      <c r="A2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="3">
-        <v>9311555369</v>
+        <v>12</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="3">
-        <v>400016</v>
+        <v>14</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="G2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>13</v>
+      <c r="J2" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>